<commit_message>
Clean up tables and code (typos, sig figs, etc)
</commit_message>
<xml_diff>
--- a/Summary Statistics for Samples.xlsx
+++ b/Summary Statistics for Samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hazenandsawyer-my.sharepoint.com/personal/bstanford_hazenandsawyer_com/Documents/00 Projects/Loxahatchee DBF Evaluation/Loxahatchee Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{1DAC3301-C263-432E-BB03-9B858262E020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CC3A89AC-7CB5-41C0-B0C4-B8F8B3A24F2E}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{1DAC3301-C263-432E-BB03-9B858262E020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C14E054-4FB7-4485-A4FC-F18B9B0BA526}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B073908D-610E-44EC-AF8E-0D1538E160A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B073908D-610E-44EC-AF8E-0D1538E160A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Influent TBF SMF" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -198,15 +198,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8E1B0D-B3D9-4277-B3B2-8D68137375E3}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B88EAD8-97CC-4135-8268-3F649C5FB824}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2066,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,10 +2131,10 @@
       <c r="D2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>18</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>11</v>
       </c>
       <c r="G2" s="2">
@@ -2163,10 +2166,10 @@
       <c r="D3" s="2">
         <v>5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>18</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="2">
@@ -2198,10 +2201,10 @@
       <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>18</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="2">
@@ -2233,10 +2236,10 @@
       <c r="D5" s="2">
         <v>0.1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="2">
@@ -2268,10 +2271,10 @@
       <c r="D6" s="2">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>18</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>5</v>
       </c>
       <c r="G6" s="2">
@@ -2303,10 +2306,10 @@
       <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>17</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>0</v>
       </c>
       <c r="G7" s="2">
@@ -2338,10 +2341,10 @@
       <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>18</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>0</v>
       </c>
       <c r="G8" s="2">
@@ -2373,10 +2376,10 @@
       <c r="D9" s="2">
         <v>0.1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="2">
@@ -2408,10 +2411,10 @@
       <c r="D10" s="2">
         <v>10</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4">
         <v>18</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <v>3</v>
       </c>
       <c r="G10" s="2">
@@ -2443,10 +2446,10 @@
       <c r="D11" s="2">
         <v>5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>18</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>2</v>
       </c>
       <c r="G11" s="2">
@@ -2478,10 +2481,10 @@
       <c r="D12" s="2">
         <v>5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>18</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>2</v>
       </c>
       <c r="G12" s="2">
@@ -2513,10 +2516,10 @@
       <c r="D13" s="2">
         <v>10</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>17</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <v>0</v>
       </c>
       <c r="G13" s="2">
@@ -2548,10 +2551,10 @@
       <c r="D14" s="2">
         <v>10</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>18</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>0</v>
       </c>
       <c r="G14" s="2">
@@ -2580,7 +2583,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,7 +2646,7 @@
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>5</v>
       </c>
       <c r="E2" s="1">
@@ -2678,7 +2681,7 @@
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>5</v>
       </c>
       <c r="E3" s="1">
@@ -2713,7 +2716,7 @@
       <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>5</v>
       </c>
       <c r="E4" s="1">
@@ -2748,7 +2751,7 @@
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0.1</v>
       </c>
       <c r="E5" s="1">
@@ -2783,7 +2786,7 @@
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>20</v>
       </c>
       <c r="E6" s="1">
@@ -2818,7 +2821,7 @@
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
       <c r="E7" s="1">
@@ -2853,7 +2856,7 @@
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="1">
@@ -2888,7 +2891,7 @@
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>0.1</v>
       </c>
       <c r="E9" s="1">
@@ -2923,7 +2926,7 @@
       <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>10</v>
       </c>
       <c r="E10" s="1">
@@ -2958,7 +2961,7 @@
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>5</v>
       </c>
       <c r="E11" s="1">
@@ -2993,7 +2996,7 @@
       <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>5</v>
       </c>
       <c r="E12" s="1">
@@ -3028,7 +3031,7 @@
       <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>10</v>
       </c>
       <c r="E13" s="1">
@@ -3063,7 +3066,7 @@
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>10</v>
       </c>
       <c r="E14" s="1">

</xml_diff>